<commit_message>
model peut lancer les differents models algo et recuperer leurs stats de precision
</commit_message>
<xml_diff>
--- a/machine_learning/apprentissage.xlsx
+++ b/machine_learning/apprentissage.xlsx
@@ -7,7 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Detailed Reports" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Accuracy Scores" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,6 +472,11 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>loss</t>
         </is>
       </c>
@@ -483,17 +489,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>{'precision': 0.7692307692307693, 'recall': 0.6896551724137931, 'f1-score': 0.7272727272727273, 'support': 29.0}</t>
+          <t>{'precision': 0.7777777777777778, 'recall': 0.7241379310344828, 'f1-score': 0.75, 'support': 29.0}</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'precision': 0.6, 'recall': 0.6666666666666666, 'f1-score': 0.631578947368421, 'support': 18.0}</t>
+          <t>{'precision': 0.6363636363636364, 'recall': 0.7777777777777778, 'f1-score': 0.7, 'support': 18.0}</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>{'precision': 0.5, 'recall': 0.5, 'f1-score': 0.5, 'support': 2.0}</t>
+          <t>{'precision': 0.0, 'recall': 0.0, 'f1-score': 0.0, 'support': 2.0}</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -502,119 +508,306 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>0.66</v>
+        <v>0.7</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>{'precision': 0.4673076923076923, 'recall': 0.4640804597701149, 'f1-score': 0.4647129186602871, 'support': 50.0}</t>
+          <t>{'precision': 0.35353535353535354, 'recall': 0.37547892720306514, 'f1-score': 0.3625, 'support': 50.0}</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>{'precision': 0.6821538461538462, 'recall': 0.66, 'f1-score': 0.6691866028708133, 'support': 50.0}</t>
+          <t>{'precision': 0.6802020202020203, 'recall': 0.7, 'f1-score': 0.687, 'support': 50.0}</t>
         </is>
       </c>
       <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>SVM</t>
+          <t>KNN</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>{'precision': 0.75, 'recall': 0.8275862068965517, 'f1-score': 0.7868852459016393, 'support': 29.0}</t>
+          <t>{'precision': 0.7391304347826086, 'recall': 0.5862068965517241, 'f1-score': 0.6538461538461539, 'support': 29.0}</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'precision': 0.75, 'recall': 0.6666666666666666, 'f1-score': 0.7058823529411765, 'support': 18.0}</t>
+          <t>{'precision': 0.5789473684210527, 'recall': 0.6111111111111112, 'f1-score': 0.5945945945945946, 'support': 18.0}</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>{'precision': 0.5, 'recall': 0.5, 'f1-score': 0.5, 'support': 2.0}</t>
+          <t>{'precision': 0.0, 'recall': 0.0, 'f1-score': 0.0, 'support': 2.0}</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>{'precision': 0.0, 'recall': 0.0, 'f1-score': 0.0, 'support': 1.0}</t>
+          <t>{'precision': 0.3333333333333333, 'recall': 1.0, 'f1-score': 0.5, 'support': 1.0}</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0.74</v>
+        <v>0.58</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>{'precision': 0.5, 'recall': 0.4985632183908046, 'f1-score': 0.498191899710704, 'support': 50.0}</t>
+          <t>{'precision': 0.3302822273073989, 'recall': 0.4394636015325671, 'f1-score': 0.3496881496881497, 'support': 50.0}</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>{'precision': 0.725, 'recall': 0.74, 'f1-score': 0.7305110896817744, 'support': 50.0}</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr"/>
+          <t>{'precision': 0.6437833714721587, 'recall': 0.58, 'f1-score': 0.6032848232848234, 'support': 50.0}</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>{'precision': 0.0, 'recall': 0.0, 'f1-score': 0.0, 'support': 0.0}</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Random Forest</t>
+          <t>SVM</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>{'precision': 0.8148148148148148, 'recall': 0.7586206896551724, 'f1-score': 0.7857142857142857, 'support': 29.0}</t>
+          <t>{'precision': 0.7777777777777778, 'recall': 0.7241379310344828, 'f1-score': 0.75, 'support': 29.0}</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{'precision': 0.6666666666666666, 'recall': 0.7777777777777778, 'f1-score': 0.717948717948718, 'support': 18.0}</t>
+          <t>{'precision': 0.5714285714285714, 'recall': 0.6666666666666666, 'f1-score': 0.6153846153846154, 'support': 18.0}</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>{'precision': 1.0, 'recall': 0.5, 'f1-score': 0.6666666666666666, 'support': 2.0}</t>
+          <t>{'precision': 0.0, 'recall': 0.0, 'f1-score': 0.0, 'support': 2.0}</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>{'precision': 1.0, 'recall': 1.0, 'f1-score': 1.0, 'support': 1.0}</t>
+          <t>{'precision': 0.5, 'recall': 1.0, 'f1-score': 0.6666666666666666, 'support': 1.0}</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>0.76</v>
+        <v>0.68</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>{'precision': 0.8703703703703703, 'recall': 0.7590996168582376, 'f1-score': 0.7925824175824175, 'support': 50.0}</t>
+          <t>{'precision': 0.4623015873015873, 'recall': 0.5977011494252873, 'f1-score': 0.5080128205128205, 'support': 50.0}</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>{'precision': 0.7725925925925927, 'recall': 0.76, 'f1-score': 0.7608424908424909, 'support': 50.0}</t>
+          <t>{'precision': 0.6668253968253969, 'recall': 0.68, 'f1-score': 0.6698717948717949, 'support': 50.0}</t>
         </is>
       </c>
       <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
+          <t>Random Forest</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>{'precision': 0.8214285714285714, 'recall': 0.7931034482758621, 'f1-score': 0.8070175438596491, 'support': 29.0}</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>{'precision': 0.7, 'recall': 0.7777777777777778, 'f1-score': 0.7368421052631579, 'support': 18.0}</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>{'precision': 1.0, 'recall': 0.5, 'f1-score': 0.6666666666666666, 'support': 2.0}</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>{'precision': 1.0, 'recall': 1.0, 'f1-score': 1.0, 'support': 1.0}</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>{'precision': 0.8803571428571428, 'recall': 0.76772030651341, 'f1-score': 0.8026315789473684, 'support': 50.0}</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>{'precision': 0.7884285714285714, 'recall': 0.78, 'f1-score': 0.78, 'support': 50.0}</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>MLP</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>{'precision': 0.84, 'recall': 0.7241379310344828, 'f1-score': 0.7777777777777778, 'support': 29.0}</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>{'precision': 0.6842105263157895, 'recall': 0.7222222222222222, 'f1-score': 0.7027027027027027, 'support': 18.0}</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>{'precision': 0.6666666666666666, 'recall': 1.0, 'f1-score': 0.8, 'support': 2.0}</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>{'precision': 0.5, 'recall': 1.0, 'f1-score': 0.6666666666666666, 'support': 1.0}</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>{'precision': 0.5381754385964912, 'recall': 0.689272030651341, 'f1-score': 0.5894294294294294, 'support': 50.0}</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>{'precision': 0.770182456140351, 'recall': 0.74, 'f1-score': 0.7494174174174174, 'support': 50.0}</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>{'precision': 0.0, 'recall': 0.0, 'f1-score': 0.0, 'support': 0.0}</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
           <t>Neural Network</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="n">
-        <v>0.6399999856948853</v>
-      </c>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="n">
-        <v>0.7583917379379272</v>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="n">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="n">
+        <v>0.8243193030357361</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Model</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Logistic Regression</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>KNN</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.58</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>SVM</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Random Forest</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>MLP</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Neural Network</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.6800000071525574</v>
       </c>
     </row>
   </sheetData>

</xml_diff>